<commit_message>
updates to summary analysis
</commit_message>
<xml_diff>
--- a/analysis/CleanedParticipantData.xlsx
+++ b/analysis/CleanedParticipantData.xlsx
@@ -10,14 +10,14 @@
     <sheet r:id="rId1" sheetId="1" name="Sheet0"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">=Sheet0!$B$2:$O$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">=Sheet0!$B$2:$P$25</definedName>
   </definedNames>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="84">
   <si>
     <t>participant</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Tasks</t>
+  </si>
+  <si>
+    <t>Gemini</t>
   </si>
   <si>
     <t>Pid</t>
@@ -109,9 +112,6 @@
     <t>How would you rate your familiarity with Python?</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>How familiar are you with AI or large language models (LLMs) like ChatGPT or Gemini?</t>
   </si>
   <si>
@@ -238,7 +238,7 @@
     <t>Data Science</t>
   </si>
   <si>
-    <t>Task 7</t>
+    <t>Task 4</t>
   </si>
   <si>
     <t>Task5</t>
@@ -294,13 +294,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -342,6 +348,13 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFc6c6c6"/>
       </left>
@@ -356,71 +369,64 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
@@ -725,30 +731,31 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="15" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="16" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="16" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="17" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="18" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="17" width="69.7192857142857" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="17" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="17" width="23.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="17" width="46.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="17" width="39.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="17" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="17" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="17" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="17" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="17" width="66.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="15" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="15" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="16" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="17" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="16" width="69.7192857142857" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="16" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="16" width="23.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="16" width="46.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="16" width="39.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="18" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="18" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="18" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="16" width="66.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -782,66 +789,62 @@
       <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="487.5">
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="834.75">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" s="3" t="s">
+      <c r="K2" s="5"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="7">
+      <c r="A3" s="1">
         <v>100</v>
       </c>
       <c r="B3" s="8">
@@ -874,21 +877,24 @@
       <c r="K3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="7">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
         <v>100</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="P3" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
-      <c r="A4" s="12">
+      <c r="A4" s="11">
         <v>110</v>
       </c>
       <c r="B4" s="8">
@@ -921,21 +927,24 @@
       <c r="K4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="7">
+        <v>13</v>
+      </c>
+      <c r="M4" s="1">
         <v>110</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="O4" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="P4" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
-      <c r="A5" s="12">
+      <c r="A5" s="11">
         <v>120</v>
       </c>
       <c r="B5" s="8">
@@ -968,21 +977,24 @@
       <c r="K5" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="7">
+        <v>25</v>
+      </c>
+      <c r="M5" s="1">
         <v>120</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="N5" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="O5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="P5" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="28.5">
-      <c r="A6" s="12">
+      <c r="A6" s="11">
         <v>130</v>
       </c>
       <c r="B6" s="8">
@@ -1015,21 +1027,24 @@
       <c r="K6" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="7">
+        <v>4</v>
+      </c>
+      <c r="M6" s="1">
         <v>130</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="N6" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="O6" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="P6" s="9" t="s">
         <v>53</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
-      <c r="A7" s="12">
+      <c r="A7" s="11">
         <v>150</v>
       </c>
       <c r="B7" s="8">
@@ -1062,21 +1077,24 @@
       <c r="K7" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="7">
+        <v>28</v>
+      </c>
+      <c r="M7" s="1">
         <v>150</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="N7" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="O7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="O7" s="9" t="s">
+      <c r="P7" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
-      <c r="A8" s="12">
+      <c r="A8" s="11">
         <v>160</v>
       </c>
       <c r="B8" s="8">
@@ -1109,21 +1127,24 @@
       <c r="K8" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="7">
+        <v>7</v>
+      </c>
+      <c r="M8" s="1">
         <v>160</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="N8" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="O8" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="O8" s="9" t="s">
+      <c r="P8" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
-      <c r="A9" s="12">
+      <c r="A9" s="11">
         <v>170</v>
       </c>
       <c r="B9" s="8">
@@ -1156,21 +1177,24 @@
       <c r="K9" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="7">
+        <v>19</v>
+      </c>
+      <c r="M9" s="1">
         <v>170</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="N9" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="O9" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="O9" s="9" t="s">
+      <c r="P9" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
-      <c r="A10" s="13">
+      <c r="A10" s="12">
         <v>180</v>
       </c>
       <c r="B10" s="8">
@@ -1203,134 +1227,143 @@
       <c r="K10" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="7">
+        <v>30</v>
+      </c>
+      <c r="M10" s="1">
         <v>180</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="N10" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="O10" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="O10" s="9" t="s">
+      <c r="P10" s="9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
-      <c r="A11" s="13">
-        <v>210</v>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="51">
+      <c r="A11" s="12">
+        <v>220</v>
       </c>
       <c r="B11" s="8">
-        <v>45713.54702546296</v>
+        <v>45713.60594907407</v>
       </c>
       <c r="C11" s="8">
-        <v>45713.548125</v>
+        <v>45713.60689814815</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" s="7">
+        <v>2</v>
+      </c>
+      <c r="M11" s="1">
+        <v>220</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="P11" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+      <c r="A12" s="12">
+        <v>230</v>
+      </c>
+      <c r="B12" s="8">
+        <v>45715.57861111111</v>
+      </c>
+      <c r="C12" s="8">
+        <v>45715.57915509259</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="J12" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="K11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L11" s="11">
-        <v>210</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="O11" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="51">
-      <c r="A12" s="13">
-        <v>220</v>
-      </c>
-      <c r="B12" s="8">
-        <v>45713.60594907407</v>
-      </c>
-      <c r="C12" s="8">
-        <v>45713.60689814815</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>54</v>
-      </c>
       <c r="K12" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L12" s="11">
-        <v>220</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="L12" s="7">
+        <v>14</v>
+      </c>
+      <c r="M12" s="1">
+        <v>230</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="O12" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
-      <c r="A13" s="13">
-        <v>230</v>
+      <c r="A13" s="12">
+        <v>240</v>
       </c>
       <c r="B13" s="8">
-        <v>45715.57861111111</v>
+        <v>45715.64090277778</v>
       </c>
       <c r="C13" s="8">
-        <v>45715.57915509259</v>
+        <v>45715.641493055555</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>29</v>
@@ -1342,45 +1375,48 @@
         <v>31</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="L13" s="11">
-        <v>230</v>
-      </c>
-      <c r="M13" s="5" t="s">
-        <v>46</v>
+        <v>67</v>
+      </c>
+      <c r="L13" s="7">
+        <v>26</v>
+      </c>
+      <c r="M13" s="1">
+        <v>240</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="O13" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="P13" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
-      <c r="A14" s="13">
-        <v>240</v>
+      <c r="A14" s="11">
+        <v>250</v>
       </c>
       <c r="B14" s="8">
-        <v>45715.64090277778</v>
+        <v>45716.47788194445</v>
       </c>
       <c r="C14" s="8">
-        <v>45715.641493055555</v>
+        <v>45716.47866898148</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="I14" s="9" t="s">
         <v>30</v>
@@ -1389,36 +1425,39 @@
         <v>31</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="L14" s="11">
-        <v>240</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>59</v>
+        <v>68</v>
+      </c>
+      <c r="L14" s="7">
+        <v>5</v>
+      </c>
+      <c r="M14" s="1">
+        <v>250</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="O14" s="9" t="s">
-        <v>35</v>
+        <v>69</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="P14" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
-      <c r="A15" s="12">
-        <v>250</v>
+      <c r="A15" s="11">
+        <v>260</v>
       </c>
       <c r="B15" s="8">
-        <v>45716.47788194445</v>
+        <v>45716.586851851855</v>
       </c>
       <c r="C15" s="8">
-        <v>45716.47866898148</v>
+        <v>45716.58756944445</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>26</v>
@@ -1427,186 +1466,198 @@
         <v>37</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="L15" s="11">
-        <v>250</v>
-      </c>
-      <c r="M15" s="5" t="s">
-        <v>69</v>
+        <v>55</v>
+      </c>
+      <c r="L15" s="7">
+        <v>17</v>
+      </c>
+      <c r="M15" s="1">
+        <v>260</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="O15" s="9" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P15" s="9" t="s">
+        <v>64</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
       <c r="A16" s="12">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="B16" s="8">
-        <v>45716.586851851855</v>
+        <v>45719.575219907405</v>
       </c>
       <c r="C16" s="8">
-        <v>45716.58756944445</v>
+        <v>45719.57556712963</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="I16" s="9" t="s">
         <v>39</v>
       </c>
       <c r="J16" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="L16" s="7">
+        <v>20</v>
+      </c>
+      <c r="M16" s="1">
+        <v>270</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="P16" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+      <c r="A17" s="12">
+        <v>280</v>
+      </c>
+      <c r="B17" s="8">
+        <v>45719.59307870371</v>
+      </c>
+      <c r="C17" s="8">
+        <v>45719.59386574074</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J17" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="K16" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="L16" s="11">
-        <v>260</v>
-      </c>
-      <c r="M16" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="N16" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="O16" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
-      <c r="A17" s="13">
-        <v>270</v>
-      </c>
-      <c r="B17" s="8">
-        <v>45719.575219907405</v>
-      </c>
-      <c r="C17" s="8">
-        <v>45719.57556712963</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J17" s="9" t="s">
-        <v>54</v>
-      </c>
       <c r="K17" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="L17" s="11">
-        <v>270</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
+      </c>
+      <c r="L17" s="7">
+        <v>11</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="O17" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="O17" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="P17" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
       <c r="A18" s="13">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="B18" s="8">
-        <v>45719.59307870371</v>
+        <v>45719.69185185185</v>
       </c>
       <c r="C18" s="8">
-        <v>45719.59386574074</v>
+        <v>45719.69265046297</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>29</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="M18" s="5" t="s">
-        <v>78</v>
+        <v>32</v>
+      </c>
+      <c r="L18" s="7">
+        <v>12</v>
+      </c>
+      <c r="M18" s="1">
+        <v>290</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="O18" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="O18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P18" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
-      <c r="A19" s="14">
-        <v>290</v>
+      <c r="A19" s="13">
+        <v>300</v>
       </c>
       <c r="B19" s="8">
-        <v>45719.69185185185</v>
+        <v>45719.70925925926</v>
       </c>
       <c r="C19" s="8">
-        <v>45719.69265046297</v>
+        <v>45719.70990740741</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>26</v>
@@ -1621,33 +1672,36 @@
         <v>30</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L19" s="11">
-        <v>290</v>
-      </c>
-      <c r="M19" s="5" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+      <c r="L19" s="7">
+        <v>24</v>
+      </c>
+      <c r="M19" s="1">
+        <v>300</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="O19" s="9" t="s">
-        <v>53</v>
+        <v>41</v>
+      </c>
+      <c r="O19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="P19" s="9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
-      <c r="A20" s="14">
-        <v>300</v>
+      <c r="A20" s="1">
+        <v>310</v>
       </c>
       <c r="B20" s="8">
-        <v>45719.70925925926</v>
+        <v>45720.55021990741</v>
       </c>
       <c r="C20" s="8">
-        <v>45719.70990740741</v>
+        <v>45720.55065972222</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>26</v>
@@ -1659,7 +1713,7 @@
         <v>26</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>29</v>
@@ -1668,33 +1722,36 @@
         <v>30</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L20" s="11">
-        <v>300</v>
-      </c>
-      <c r="M20" s="5" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="L20" s="7">
+        <v>3</v>
+      </c>
+      <c r="M20" s="1">
+        <v>310</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="O20" s="9" t="s">
-        <v>35</v>
+        <v>46</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="P20" s="9" t="s">
+        <v>64</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
-      <c r="A21" s="7">
-        <v>310</v>
+      <c r="A21" s="1">
+        <v>330</v>
       </c>
       <c r="B21" s="8">
-        <v>45720.55021990741</v>
+        <v>45728.62128472222</v>
       </c>
       <c r="C21" s="8">
-        <v>45720.55065972222</v>
+        <v>45728.62207175926</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>26</v>
@@ -1706,7 +1763,7 @@
         <v>26</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>29</v>
@@ -1715,33 +1772,36 @@
         <v>30</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="L21" s="11">
-        <v>310</v>
-      </c>
-      <c r="M21" s="5" t="s">
-        <v>46</v>
+        <v>68</v>
+      </c>
+      <c r="L21" s="7">
+        <v>27</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="N21" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="O21" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="O21" s="9" t="s">
-        <v>64</v>
+      <c r="P21" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
-      <c r="A22" s="14">
-        <v>320</v>
+      <c r="A22" s="13">
+        <v>340</v>
       </c>
       <c r="B22" s="8">
-        <v>45722.50326388889</v>
+        <v>45733.70077546296</v>
       </c>
       <c r="C22" s="8">
-        <v>45722.50409722222</v>
+        <v>45733.70145833334</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>26</v>
@@ -1762,86 +1822,92 @@
         <v>30</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="L22" s="11">
-        <v>320</v>
-      </c>
-      <c r="M22" s="5" t="s">
-        <v>51</v>
+        <v>55</v>
+      </c>
+      <c r="L22" s="7">
+        <v>6</v>
+      </c>
+      <c r="M22" s="1">
+        <v>340</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="O22" s="9" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+      <c r="O22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P22" s="9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
-      <c r="A23" s="7">
-        <v>330</v>
+      <c r="A23" s="1">
+        <v>350</v>
       </c>
       <c r="B23" s="8">
-        <v>45728.62128472222</v>
+        <v>45734.62398148148</v>
       </c>
       <c r="C23" s="8">
-        <v>45728.62207175926</v>
+        <v>45734.62509259259</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="H23" s="9" t="s">
         <v>29</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="J23" s="9" t="s">
         <v>81</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="M23" s="5" t="s">
-        <v>69</v>
+        <v>58</v>
+      </c>
+      <c r="L23" s="7">
+        <v>18</v>
+      </c>
+      <c r="M23" s="1">
+        <v>350</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="O23" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="O23" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="P23" s="9" t="s">
         <v>53</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
-      <c r="A24" s="14">
-        <v>340</v>
+      <c r="A24" s="13">
+        <v>360</v>
       </c>
       <c r="B24" s="8">
-        <v>45733.70077546296</v>
+        <v>45736.64690972222</v>
       </c>
       <c r="C24" s="8">
-        <v>45733.70145833334</v>
+        <v>45736.647523148145</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>26</v>
@@ -1850,121 +1916,30 @@
         <v>37</v>
       </c>
       <c r="H24" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L24" s="7">
         <v>29</v>
       </c>
-      <c r="I24" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="J24" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="K24" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="L24" s="11">
-        <v>340</v>
-      </c>
-      <c r="M24" s="5" t="s">
-        <v>56</v>
+      <c r="M24" s="1">
+        <v>360</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="O24" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
-      <c r="A25" s="7">
-        <v>350</v>
-      </c>
-      <c r="B25" s="8">
-        <v>45734.62398148148</v>
-      </c>
-      <c r="C25" s="8">
-        <v>45734.62509259259</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I25" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="J25" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L25" s="11">
-        <v>350</v>
-      </c>
-      <c r="M25" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="N25" s="5" t="s">
+      <c r="O24" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="O25" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
-      <c r="A26" s="14">
-        <v>360</v>
-      </c>
-      <c r="B26" s="8">
-        <v>45736.64690972222</v>
-      </c>
-      <c r="C26" s="8">
-        <v>45736.647523148145</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="I26" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J26" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L26" s="11">
-        <v>360</v>
-      </c>
-      <c r="M26" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="N26" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="O26" s="9" t="s">
+      <c r="P24" s="9" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>